<commit_message>
version 1.1.1 tablas 5 a 8 nom 10
</commit_message>
<xml_diff>
--- a/data_sets/template_tabla.xlsx
+++ b/data_sets/template_tabla.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2dbb1e87085fa55/Estudios/ESTUDIOS2024/NOM005Bitron24/proyecto/data_sets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{2D4EC983-FF0C-2347-8176-A5B7978DF6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D355775F-47EB-B943-BA14-0D0C6728EEFF}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:1_{2D4EC983-FF0C-2347-8176-A5B7978DF6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B38ABC9-DAF8-774D-808A-DF84BE3CD445}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Archivo</t>
   </si>
@@ -163,20 +176,41 @@
     <t xml:space="preserve">Valores Límite de Exposición </t>
   </si>
   <si>
-    <t>Oral</t>
-  </si>
-  <si>
-    <t>Cutanea</t>
-  </si>
-  <si>
-    <t>Inhalación</t>
+    <t>Oral Valor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oral Unidades </t>
+  </si>
+  <si>
+    <t>Inhalacion Valor</t>
+  </si>
+  <si>
+    <t>Inhalacion Unidades</t>
+  </si>
+  <si>
+    <t>Cutanea Valor</t>
+  </si>
+  <si>
+    <t>Cutanea Unidades</t>
+  </si>
+  <si>
+    <t>Riesgo Tabla 5</t>
+  </si>
+  <si>
+    <t>NOM-010-STPS</t>
+  </si>
+  <si>
+    <t>Volatilidad Tabla 7 y 8</t>
+  </si>
+  <si>
+    <t>Peligro Tabla 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +233,41 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -275,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -283,12 +352,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -302,13 +383,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -613,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BB8"/>
+  <dimension ref="A1:BH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AV10" sqref="AV10"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" zoomScale="215" zoomScaleNormal="215" workbookViewId="0">
+      <selection activeCell="BH2" sqref="BH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -644,249 +728,279 @@
     <col min="33" max="46" width="6" customWidth="1"/>
     <col min="47" max="48" width="20" customWidth="1"/>
     <col min="49" max="51" width="8" customWidth="1"/>
+    <col min="52" max="53" width="6.83203125" customWidth="1"/>
+    <col min="54" max="55" width="7.1640625" customWidth="1"/>
+    <col min="56" max="57" width="6.83203125" customWidth="1"/>
+    <col min="58" max="60" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:60" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="6" t="s">
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AD1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AE1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="6" t="s">
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="AH1" s="7"/>
-      <c r="AI1" s="6" t="s">
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="AJ1" s="7"/>
-      <c r="AK1" s="6" t="s">
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AL1" s="7"/>
-      <c r="AM1" s="6" t="s">
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AN1" s="7"/>
-      <c r="AO1" s="6" t="s">
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AP1" s="7"/>
-      <c r="AQ1" s="6" t="s">
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AR1" s="7"/>
-      <c r="AS1" s="6" t="s">
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AT1" s="7"/>
-      <c r="AU1" s="6" t="s">
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="AV1" s="6" t="s">
+      <c r="AV1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AW1" s="6" t="s">
+      <c r="AW1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="AX1" s="6" t="s">
+      <c r="AX1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AY1" s="6" t="s">
+      <c r="AY1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AZ1" s="10" t="s">
+      <c r="AZ1" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="14"/>
+      <c r="BC1" s="14"/>
+      <c r="BD1" s="14"/>
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="BG1" s="16"/>
+      <c r="BH1" s="16"/>
     </row>
-    <row r="2" spans="1:54" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="3" t="s">
+    <row r="2" spans="1:60" s="2" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="5" t="s">
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AF2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AG2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AH2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AI2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AK2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AL2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AM2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AN2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AO2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AP2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AR2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AS2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AT2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AU2" s="6"/>
-      <c r="AV2" s="6"/>
-      <c r="AW2" s="6"/>
-      <c r="AX2" s="6"/>
-      <c r="AY2" s="6"/>
-      <c r="AZ2" s="11" t="s">
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="10"/>
+      <c r="AX2" s="10"/>
+      <c r="AY2" s="10"/>
+      <c r="AZ2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="BA2" s="11" t="s">
+      <c r="BA2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="BB2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="BB2" s="11" t="s">
-        <v>48</v>
+      <c r="BC2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="BE2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="BF2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="BG2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BH2" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -919,19 +1033,40 @@
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
       <c r="AY3" s="1"/>
+      <c r="AZ3" s="1"/>
     </row>
-    <row r="6" spans="1:54" ht="16" x14ac:dyDescent="0.2">
-      <c r="P6" s="4"/>
+    <row r="6" spans="1:60" ht="16" x14ac:dyDescent="0.2">
+      <c r="P6" s="3"/>
     </row>
-    <row r="7" spans="1:54" ht="16" x14ac:dyDescent="0.2">
-      <c r="P7" s="4"/>
+    <row r="7" spans="1:60" ht="16" x14ac:dyDescent="0.2">
+      <c r="P7" s="3"/>
     </row>
-    <row r="8" spans="1:54" ht="16" x14ac:dyDescent="0.2">
-      <c r="P8" s="4"/>
+    <row r="8" spans="1:60" ht="16" x14ac:dyDescent="0.2">
+      <c r="P8" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="AZ1:BB1"/>
+  <mergeCells count="37">
+    <mergeCell ref="AZ1:BE1"/>
+    <mergeCell ref="BF1:BH1"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="AU1:AU2"/>
+    <mergeCell ref="AV1:AV2"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AS1:AT1"/>
+    <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AW1:AW2"/>
     <mergeCell ref="AX1:AX2"/>
     <mergeCell ref="AY1:AY2"/>
@@ -947,26 +1082,7 @@
     <mergeCell ref="AO1:AP1"/>
     <mergeCell ref="AI1:AJ1"/>
     <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AC1:AC2"/>
     <mergeCell ref="AD1:AD2"/>
-    <mergeCell ref="AU1:AU2"/>
-    <mergeCell ref="AV1:AV2"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="AS1:AT1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="O1:O2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>